<commit_message>
Update CAPS TESTING RESULT V.1.3.1.xlsx
</commit_message>
<xml_diff>
--- a/TESTING ENVIRONMENT RESULTS/CAPS TESTING RESULT V.1.3.1.xlsx
+++ b/TESTING ENVIRONMENT RESULTS/CAPS TESTING RESULT V.1.3.1.xlsx
@@ -58,9 +58,6 @@
     <t>SET UP EXAM FOR PRACTICE QUESTION</t>
   </si>
   <si>
-    <t>Internal orror occured is the output</t>
-  </si>
-  <si>
     <t>ADD SUBJECT</t>
   </si>
   <si>
@@ -101,6 +98,9 @@
   </si>
   <si>
     <t>TAKE PRACTICE EXAM</t>
+  </si>
+  <si>
+    <t>I CAN ACCESS QUALIFYING EXAM QUESTIONS IF I ANSWER  IN PRACTICE EXAM</t>
   </si>
   <si>
     <t>SEE SCORE AFTER TAKING THE EXAM</t>
@@ -433,7 +433,8 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="25.38"/>
     <col customWidth="1" min="2" max="2" width="62.13"/>
-    <col customWidth="1" min="4" max="4" width="29.38"/>
+    <col customWidth="1" min="3" max="3" width="11.88"/>
+    <col customWidth="1" min="4" max="4" width="67.88"/>
     <col customWidth="1" min="7" max="7" width="14.38"/>
   </cols>
   <sheetData>
@@ -542,10 +543,8 @@
       <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="6"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -553,7 +552,7 @@
     <row r="10">
       <c r="A10" s="1"/>
       <c r="B10" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="3"/>
@@ -564,7 +563,7 @@
     <row r="11">
       <c r="A11" s="3"/>
       <c r="B11" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="3"/>
@@ -575,7 +574,7 @@
     <row r="12">
       <c r="A12" s="1"/>
       <c r="B12" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="6"/>
@@ -586,11 +585,11 @@
     <row r="13">
       <c r="A13" s="1"/>
       <c r="B13" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -607,7 +606,7 @@
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>4</v>
@@ -632,7 +631,7 @@
     <row r="17">
       <c r="A17" s="3"/>
       <c r="B17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="3"/>
@@ -665,7 +664,7 @@
     <row r="20">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="3"/>
@@ -687,7 +686,7 @@
     <row r="22">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="3"/>
@@ -706,10 +705,10 @@
     </row>
     <row r="24">
       <c r="A24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="3"/>
@@ -720,7 +719,7 @@
     <row r="25">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="3"/>
@@ -731,7 +730,7 @@
     <row r="26">
       <c r="A26" s="1"/>
       <c r="B26" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="3"/>
@@ -742,7 +741,7 @@
     <row r="27">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="3"/>
@@ -761,13 +760,15 @@
     </row>
     <row r="29">
       <c r="A29" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="C29" s="5"/>
+      <c r="D29" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -777,7 +778,7 @@
       <c r="B30" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="1"/>
+      <c r="C30" s="7"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -788,7 +789,7 @@
       <c r="B31" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="1"/>
+      <c r="C31" s="7"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>

</xml_diff>